<commit_message>
some testing changes to revert back
</commit_message>
<xml_diff>
--- a/target/classes/join.xlsx
+++ b/target/classes/join.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>Title</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Passed</t>
+  </si>
+  <si>
+    <t>Failed</t>
   </si>
 </sst>
 </file>
@@ -176,7 +179,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +209,21 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
     </font>
   </fonts>
   <fills count="4">
@@ -241,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -254,6 +272,15 @@
       <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment wrapText="true"/>
     </xf>
   </cellXfs>
@@ -653,8 +680,8 @@
       <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" t="s" s="5">
-        <v>44</v>
+      <c r="J3" t="s" s="8">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -685,8 +712,8 @@
       <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s" s="6">
-        <v>44</v>
+      <c r="J4" t="s" s="9">
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -717,8 +744,8 @@
       <c r="I5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" t="s" s="7">
-        <v>44</v>
+      <c r="J5" t="s" s="10">
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>